<commit_message>
call of the methods in Main was changed, methods atrs were fixed
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="197">
   <si>
     <t>Пациент</t>
   </si>
@@ -92,7 +92,7 @@
     <t>105</t>
   </si>
   <si>
-    <t>euroscore&lt;5 5-10 &gt;10</t>
+    <t>euroscore&lt;5 5.10 &gt;10</t>
   </si>
   <si>
     <t>0.8</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve"> 2</t>
   </si>
   <si>
-    <t>STS score &lt;3 3-8 &gt;8</t>
+    <t>STS score &lt;3 3.8 &gt;8</t>
   </si>
   <si>
     <t>0.6</t>
@@ -128,7 +128,7 @@
     <t>S АоКл</t>
   </si>
   <si>
-    <t>0, 92</t>
+    <t>0. 92</t>
   </si>
   <si>
     <t>аортальная регургитация</t>
@@ -197,36 +197,72 @@
     <t>21</t>
   </si>
   <si>
+    <t>Нарушения ритма</t>
+  </si>
+  <si>
     <t>80</t>
   </si>
   <si>
+    <t>ОИМ</t>
+  </si>
+  <si>
     <t>89</t>
   </si>
   <si>
+    <t>Повторная реваскуляризация</t>
+  </si>
+  <si>
+    <t>ОНМК</t>
+  </si>
+  <si>
     <t>115</t>
   </si>
   <si>
+    <t>Смерть</t>
+  </si>
+  <si>
+    <t>МАССЕ</t>
+  </si>
+  <si>
     <t>103</t>
   </si>
   <si>
+    <t>ОПН</t>
+  </si>
+  <si>
     <t>101</t>
   </si>
   <si>
+    <t>Кровотечения</t>
+  </si>
+  <si>
     <t>109</t>
   </si>
   <si>
+    <t>кол.во шунтов</t>
+  </si>
+  <si>
     <t>58</t>
   </si>
   <si>
+    <t>Тип стента</t>
+  </si>
+  <si>
     <t>bms</t>
   </si>
   <si>
     <t>64</t>
   </si>
   <si>
+    <t>полная неполна реваск</t>
+  </si>
+  <si>
     <t>65</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>01.05.2014</t>
   </si>
   <si>
@@ -236,9 +272,6 @@
     <t>11</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>PCI</t>
   </si>
   <si>
@@ -272,7 +305,7 @@
     <t>34</t>
   </si>
   <si>
-    <t>0,5</t>
+    <t>0.5</t>
   </si>
   <si>
     <t xml:space="preserve"> 4</t>
@@ -365,7 +398,7 @@
     <t>35</t>
   </si>
   <si>
-    <t>0,58</t>
+    <t>0.58</t>
   </si>
   <si>
     <t>67</t>
@@ -413,7 +446,7 @@
     <t>36</t>
   </si>
   <si>
-    <t>0,59</t>
+    <t>0.59</t>
   </si>
   <si>
     <t>29</t>
@@ -449,9 +482,6 @@
     <t>62</t>
   </si>
   <si>
-    <t>0,6</t>
-  </si>
-  <si>
     <t>02.02.2010</t>
   </si>
   <si>
@@ -476,7 +506,7 @@
     <t>63</t>
   </si>
   <si>
-    <t>0,65</t>
+    <t>0.65</t>
   </si>
   <si>
     <t>02.03.2012</t>
@@ -500,7 +530,7 @@
     <t>39</t>
   </si>
   <si>
-    <t>0,7</t>
+    <t>0.7</t>
   </si>
   <si>
     <t>02.09.2014</t>
@@ -521,7 +551,7 @@
     <t>1.38</t>
   </si>
   <si>
-    <t>0,75</t>
+    <t>0.75</t>
   </si>
   <si>
     <t>02.10.2013</t>
@@ -551,7 +581,7 @@
     <t>41</t>
   </si>
   <si>
-    <t>0,78</t>
+    <t>0.78</t>
   </si>
   <si>
     <t>02.12.2014</t>
@@ -564,9 +594,6 @@
   </si>
   <si>
     <t>1.56</t>
-  </si>
-  <si>
-    <t>0,8</t>
   </si>
   <si>
     <t>03.02.2011</t>
@@ -724,31 +751,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J1" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2">
@@ -756,31 +783,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3">
@@ -788,31 +815,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J3" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
@@ -820,31 +847,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5">
@@ -855,28 +882,28 @@
         <v>34</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s" s="3">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J5" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
@@ -887,28 +914,28 @@
         <v>49</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E6" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F6" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H6" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I6" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
@@ -916,31 +943,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J7" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
@@ -948,25 +975,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s" s="3">
+        <v>130</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>151</v>
+      </c>
+      <c r="F8" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="G8" t="s" s="3">
         <v>119</v>
       </c>
-      <c r="E8" t="s" s="3">
-        <v>140</v>
-      </c>
-      <c r="F8" t="s" s="3">
-        <v>150</v>
-      </c>
-      <c r="G8" t="s" s="3">
-        <v>108</v>
-      </c>
       <c r="H8" t="s" s="3">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="I8" t="s" s="3">
         <v>45</v>
@@ -1012,31 +1039,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J10" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
@@ -1044,31 +1071,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s" s="3">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="F11" t="s" s="3">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G11" t="s" s="3">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="H11" t="s" s="3">
         <v>49</v>
       </c>
       <c r="I11" t="s" s="3">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="J11" t="s" s="3">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12">
@@ -1108,31 +1135,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J13" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
@@ -1143,28 +1170,28 @@
         <v>34</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G14" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H14" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I14" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J14" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15">
@@ -1172,31 +1199,31 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="E15" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G15" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J15" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -1204,31 +1231,31 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J16" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -1239,28 +1266,28 @@
         <v>31</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J17" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
@@ -1268,31 +1295,31 @@
         <v>15</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J18" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
@@ -1300,31 +1327,31 @@
         <v>16</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J19" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20">
@@ -1335,28 +1362,28 @@
         <v>34</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J20" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21">
@@ -1364,31 +1391,31 @@
         <v>17</v>
       </c>
       <c r="B21" t="s" s="3">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J21" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22">
@@ -1396,31 +1423,31 @@
         <v>18</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J22" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23">
@@ -1437,22 +1464,22 @@
         <v>31</v>
       </c>
       <c r="E23" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G23" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H23" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I23" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J23" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24">
@@ -1466,25 +1493,25 @@
         <v>15</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="E24" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G24" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H24" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I24" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J24" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25">
@@ -1492,31 +1519,31 @@
         <v>20</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J25" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26">
@@ -1527,28 +1554,28 @@
         <v>34</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J26" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27">
@@ -1556,31 +1583,31 @@
         <v>21</v>
       </c>
       <c r="B27" t="s" s="3">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J27" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28">
@@ -1588,31 +1615,31 @@
         <v>22</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J28" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29">
@@ -1623,28 +1650,28 @@
         <v>34</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J29" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30">
@@ -1652,31 +1679,31 @@
         <v>23</v>
       </c>
       <c r="B30" t="s" s="3">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J30" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31">
@@ -1684,31 +1711,31 @@
         <v>24</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J31" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32">
@@ -1719,28 +1746,28 @@
         <v>34</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J32" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33">
@@ -1748,31 +1775,31 @@
         <v>25</v>
       </c>
       <c r="B33" t="s" s="3">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J33" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34">
@@ -1780,31 +1807,31 @@
         <v>26</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J34" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35">
@@ -1815,28 +1842,28 @@
         <v>34</v>
       </c>
       <c r="C35" t="s" s="3">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="D35" t="s" s="3">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="E35" t="s" s="3">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="F35" t="s" s="3">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="G35" t="s" s="3">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="H35" t="s" s="3">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="I35" t="s" s="3">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="J35" t="s" s="3">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36">
@@ -1856,10 +1883,10 @@
         <v>8</v>
       </c>
       <c r="F36" t="s" s="3">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s" s="3">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="H36" t="s" s="3">
         <v>8</v>
@@ -1876,31 +1903,31 @@
         <v>29</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J37" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38">
@@ -1911,28 +1938,28 @@
         <v>27</v>
       </c>
       <c r="C38" t="s" s="3">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s" s="3">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E38" t="s" s="3">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="F38" t="s" s="3">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="G38" t="s" s="3">
         <v>34</v>
       </c>
       <c r="H38" t="s" s="3">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="I38" t="s" s="3">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="J38" t="s" s="3">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39">
@@ -1943,7 +1970,7 @@
         <v>31</v>
       </c>
       <c r="C39" t="s" s="3">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D39" t="s" s="3">
         <v>34</v>
@@ -1955,16 +1982,16 @@
         <v>34</v>
       </c>
       <c r="G39" t="s" s="3">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="H39" t="s" s="3">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="I39" t="s" s="3">
         <v>34</v>
       </c>
       <c r="J39" t="s" s="3">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40">
@@ -1972,31 +1999,31 @@
         <v>32</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J40" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41">
@@ -2004,31 +2031,31 @@
         <v>33</v>
       </c>
       <c r="B41" t="s" s="3">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s" s="3">
         <v>49</v>
       </c>
       <c r="D41" t="s" s="3">
+        <v>140</v>
+      </c>
+      <c r="E41" t="s" s="3">
+        <v>155</v>
+      </c>
+      <c r="F41" t="s" s="3">
+        <v>163</v>
+      </c>
+      <c r="G41" t="s" s="3">
+        <v>79</v>
+      </c>
+      <c r="H41" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="I41" t="s" s="3">
+        <v>187</v>
+      </c>
+      <c r="J41" t="s" s="3">
         <v>129</v>
-      </c>
-      <c r="E41" t="s" s="3">
-        <v>144</v>
-      </c>
-      <c r="F41" t="s" s="3">
-        <v>153</v>
-      </c>
-      <c r="G41" t="s" s="3">
-        <v>69</v>
-      </c>
-      <c r="H41" t="s" s="3">
-        <v>70</v>
-      </c>
-      <c r="I41" t="s" s="3">
-        <v>177</v>
-      </c>
-      <c r="J41" t="s" s="3">
-        <v>118</v>
       </c>
     </row>
     <row r="42">
@@ -2060,7 +2087,7 @@
         <v>11</v>
       </c>
       <c r="J42" t="s" s="3">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43">
@@ -2068,31 +2095,31 @@
         <v>35</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J43" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44">
@@ -2100,31 +2127,31 @@
         <v>36</v>
       </c>
       <c r="B44" t="s" s="3">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s" s="3">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D44" t="s" s="3">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="E44" t="s" s="3">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="F44" t="s" s="3">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="G44" t="s" s="3">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="H44" t="s" s="3">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="I44" t="s" s="3">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="J44" t="s" s="3">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45">
@@ -2141,13 +2168,13 @@
         <v>58</v>
       </c>
       <c r="E45" t="s" s="3">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="F45" t="s" s="3">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="G45" t="s" s="3">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="H45" t="s" s="3">
         <v>40</v>
@@ -2164,31 +2191,31 @@
         <v>37</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J46" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47">
@@ -2196,31 +2223,31 @@
         <v>38</v>
       </c>
       <c r="B47" t="s" s="3">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s" s="3">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s" s="3">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E47" t="s" s="3">
-        <v>145</v>
+        <v>30</v>
       </c>
       <c r="F47" t="s" s="3">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="G47" t="s" s="3">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="H47" t="s" s="3">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I47" t="s" s="3">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="J47" t="s" s="3">
-        <v>184</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48">
@@ -2228,7 +2255,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s" s="3">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s" s="3">
         <v>8</v>
@@ -2243,7 +2270,7 @@
         <v>8</v>
       </c>
       <c r="G48" t="s" s="3">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="H48" t="s" s="3">
         <v>8</v>
@@ -2252,7 +2279,7 @@
         <v>28</v>
       </c>
       <c r="J48" t="s" s="3">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49">
@@ -2260,31 +2287,31 @@
         <v>39</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J49" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50">
@@ -2301,22 +2328,22 @@
         <v>31</v>
       </c>
       <c r="E50" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F50" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G50" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H50" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I50" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J50" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51">
@@ -2324,31 +2351,31 @@
         <v>40</v>
       </c>
       <c r="B51" t="s" s="3">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C51" t="s" s="3">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="D51" t="s" s="3">
         <v>8</v>
       </c>
       <c r="E51" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F51" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G51" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H51" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I51" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J51" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52">
@@ -2356,31 +2383,31 @@
         <v>41</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J52" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53">
@@ -2391,28 +2418,28 @@
         <v>11</v>
       </c>
       <c r="C53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J53" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54">
@@ -2420,31 +2447,31 @@
         <v>42</v>
       </c>
       <c r="B54" t="s" s="3">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J54" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55">
@@ -2452,31 +2479,31 @@
         <v>43</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J55" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56">
@@ -2484,31 +2511,31 @@
         <v>34</v>
       </c>
       <c r="B56" t="s" s="3">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s" s="3">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D56" t="s" s="3">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="E56" t="s" s="3">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="F56" t="s" s="3">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="G56" t="s" s="3">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="H56" t="s" s="3">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="I56" t="s" s="3">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="J56" t="s" s="3">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57">
@@ -2548,31 +2575,31 @@
         <v>44</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J58" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59">
@@ -2586,25 +2613,25 @@
         <v>11</v>
       </c>
       <c r="D59" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E59" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F59" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G59" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H59" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I59" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J59" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60">
@@ -2615,28 +2642,28 @@
         <v>5</v>
       </c>
       <c r="C60" t="s" s="3">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="D60" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E60" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F60" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G60" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H60" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I60" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J60" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61">
@@ -2644,31 +2671,31 @@
         <v>46</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J61" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62">
@@ -2682,25 +2709,25 @@
         <v>11</v>
       </c>
       <c r="D62" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E62" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F62" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G62" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H62" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I62" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J62" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63">
@@ -2708,31 +2735,31 @@
         <v>47</v>
       </c>
       <c r="B63" t="s" s="3">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s" s="3">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E63" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F63" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G63" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H63" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I63" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J63" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64">
@@ -2740,31 +2767,31 @@
         <v>48</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J64" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65">
@@ -2778,25 +2805,25 @@
         <v>11</v>
       </c>
       <c r="D65" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E65" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F65" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G65" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H65" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I65" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J65" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66">
@@ -2804,31 +2831,31 @@
         <v>49</v>
       </c>
       <c r="B66" t="s" s="3">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s" s="3">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D66" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E66" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F66" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G66" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H66" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I66" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J66" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67">
@@ -2836,31 +2863,31 @@
         <v>50</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J67" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68">
@@ -2874,25 +2901,25 @@
         <v>11</v>
       </c>
       <c r="D68" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E68" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F68" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G68" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H68" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I68" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J68" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69">
@@ -2900,31 +2927,31 @@
         <v>51</v>
       </c>
       <c r="B69" t="s" s="3">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C69" t="s" s="3">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D69" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E69" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F69" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G69" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H69" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I69" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J69" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70">
@@ -2932,31 +2959,31 @@
         <v>52</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J70" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71">
@@ -2964,31 +2991,31 @@
         <v>53</v>
       </c>
       <c r="B71" t="s" s="3">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C71" t="s" s="3">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="D71" t="s" s="3">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="E71" t="s" s="3">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F71" t="s" s="3">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="G71" t="s" s="3">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="H71" t="s" s="3">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="I71" t="s" s="3">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="J71" t="s" s="3">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72">
@@ -3028,31 +3055,31 @@
         <v>54</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J73" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74">
@@ -3060,31 +3087,31 @@
         <v>34</v>
       </c>
       <c r="B74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J74" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75">
@@ -3092,31 +3119,31 @@
         <v>55</v>
       </c>
       <c r="B75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J75" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76">
@@ -3124,31 +3151,31 @@
         <v>56</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J76" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77">
@@ -3156,10 +3183,10 @@
         <v>57</v>
       </c>
       <c r="B77" t="s" s="3">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C77" t="s" s="3">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="D77" t="s" s="3">
         <v>21</v>
@@ -3168,19 +3195,19 @@
         <v>51</v>
       </c>
       <c r="F77" t="s" s="3">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="G77" t="s" s="3">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="H77" t="s" s="3">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="I77" t="s" s="3">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="J77" t="s" s="3">
-        <v>186</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78">
@@ -3220,31 +3247,31 @@
         <v>32</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J79" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80">
@@ -3255,28 +3282,28 @@
         <v>31</v>
       </c>
       <c r="C80" t="s" s="3">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D80" t="s" s="3">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E80" t="s" s="3">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F80" t="s" s="3">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="G80" t="s" s="3">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="H80" t="s" s="3">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="I80" t="s" s="3">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="J80" t="s" s="3">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81">
@@ -3284,28 +3311,28 @@
         <v>58</v>
       </c>
       <c r="B81" t="s" s="3">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C81" t="s" s="3">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="D81" t="s" s="3">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E81" t="s" s="3">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="F81" t="s" s="3">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="G81" t="s" s="3">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="H81" t="s" s="3">
         <v>58</v>
       </c>
       <c r="I81" t="s" s="3">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="J81" t="s" s="3">
         <v>58</v>
@@ -3316,31 +3343,31 @@
         <v>35</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J82" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83">
@@ -3357,22 +3384,22 @@
         <v>31</v>
       </c>
       <c r="E83" t="s" s="3">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="F83" t="s" s="3">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="G83" t="s" s="3">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="H83" t="s" s="3">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="I83" t="s" s="3">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="J83" t="s" s="3">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84">
@@ -3383,19 +3410,19 @@
         <v>58</v>
       </c>
       <c r="C84" t="s" s="3">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D84" t="s" s="3">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="E84" t="s" s="3">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="F84" t="s" s="3">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="G84" t="s" s="3">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="H84" t="s" s="3">
         <v>40</v>
@@ -3412,31 +3439,31 @@
         <v>39</v>
       </c>
       <c r="B85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J85" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86">
@@ -3453,22 +3480,22 @@
         <v>31</v>
       </c>
       <c r="E86" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F86" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G86" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H86" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I86" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J86" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87">
@@ -3476,7 +3503,7 @@
         <v>59</v>
       </c>
       <c r="B87" t="s" s="3">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s" s="3">
         <v>58</v>
@@ -3485,118 +3512,118 @@
         <v>8</v>
       </c>
       <c r="E87" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F87" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G87" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H87" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I87" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J87" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s" s="4">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B88" t="s" s="4">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C88" t="s" s="4">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="D88" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E88" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F88" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G88" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H88" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I88" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J88" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="3">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="B89" t="s" s="3">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s" s="3">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="D89" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E89" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F89" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G89" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H89" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I89" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J89" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s" s="3">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="B90" t="s" s="3">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="C90" t="s" s="3">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="D90" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E90" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F90" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G90" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H90" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I90" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J90" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91">
@@ -3604,31 +3631,31 @@
         <v>61</v>
       </c>
       <c r="B91" t="s" s="4">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J91" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92">
@@ -3639,28 +3666,28 @@
         <v>34</v>
       </c>
       <c r="C92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J92" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93">
@@ -3668,159 +3695,159 @@
         <v>62</v>
       </c>
       <c r="B93" t="s" s="3">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="C93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J93" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s" s="4">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B94" t="s" s="4">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J94" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s" s="3">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B95" t="s" s="3">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J95" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s" s="3">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B96" t="s" s="3">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J96" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B97" t="s" s="4">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J97" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98">
@@ -3831,28 +3858,28 @@
         <v>34</v>
       </c>
       <c r="C98" t="s" s="3">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="D98" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E98" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F98" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G98" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H98" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I98" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J98" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99">
@@ -3860,159 +3887,159 @@
         <v>25</v>
       </c>
       <c r="B99" t="s" s="3">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C99" t="s" s="3">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="D99" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E99" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F99" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G99" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H99" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I99" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J99" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="4">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B100" t="s" s="4">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J100" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="3">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B101" t="s" s="3">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="C101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J101" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s" s="3">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B102" t="s" s="3">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="C102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J102" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s" s="4">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B103" t="s" s="4">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J103" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="104">
@@ -4023,188 +4050,188 @@
         <v>34</v>
       </c>
       <c r="C104" t="s" s="3">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="D104" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E104" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F104" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G104" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H104" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I104" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J104" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s" s="3">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B105" t="s" s="3">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C105" t="s" s="3">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="D105" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E105" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F105" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G105" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H105" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I105" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J105" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s" s="4">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B106" t="s" s="4">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C106" t="s" s="4">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="D106" t="s" s="4">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="E106" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F106" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G106" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H106" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I106" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J106" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s" s="3">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B107" t="s" s="3">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="C107" t="s" s="3">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="D107" t="s" s="3">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="E107" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F107" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G107" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H107" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I107" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J107" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s" s="3">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B108" t="s" s="3">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C108" t="s" s="3">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="D108" t="s" s="3">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="E108" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F108" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G108" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H108" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I108" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J108" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s" s="4">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B109" t="s" s="4">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="C109" t="s" s="4">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="D109" t="s" s="4">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E109" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F109" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G109" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H109" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I109" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J109" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="110">
@@ -4215,188 +4242,636 @@
         <v>34</v>
       </c>
       <c r="C110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J110" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B111" t="s" s="3">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J111" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s" s="4">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B112" t="s" s="4">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C112" t="s" s="4">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="D112" t="s" s="4">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E112" t="s" s="4">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="F112" t="s" s="4">
-        <v>158</v>
+        <v>82</v>
       </c>
       <c r="G112" t="s" s="4">
-        <v>166</v>
+        <v>82</v>
       </c>
       <c r="H112" t="s" s="4">
-        <v>173</v>
+        <v>82</v>
       </c>
       <c r="I112" t="s" s="4">
-        <v>182</v>
+        <v>82</v>
       </c>
       <c r="J112" t="s" s="4">
-        <v>187</v>
+        <v>82</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s" s="3">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B113" t="s" s="3">
         <v>34</v>
       </c>
       <c r="C113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="D113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="E113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="F113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="G113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="H113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="I113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="J113" t="s" s="3">
-        <v>34</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s" s="3">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B114" t="s" s="3">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J114" t="s" s="3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s" s="4">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B115" t="s" s="4">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J115" t="s" s="4">
-        <v>74</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B116" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="C116" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="D116" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="E116" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F116" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G116" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H116" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I116" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J116" t="s" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="3">
+        <v>76</v>
+      </c>
+      <c r="B117" t="s" s="3">
+        <v>114</v>
+      </c>
+      <c r="C117" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="D117" t="s" s="3">
+        <v>116</v>
+      </c>
+      <c r="E117" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F117" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G117" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H117" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I117" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J117" t="s" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="B118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="C118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="D118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="E118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="F118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="G118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="H118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="I118" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="J118" t="s" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="B119" t="s" s="3">
+        <v>115</v>
+      </c>
+      <c r="C119" t="s" s="3">
+        <v>135</v>
+      </c>
+      <c r="D119" t="s" s="3">
+        <v>149</v>
+      </c>
+      <c r="E119" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F119" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G119" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H119" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I119" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J119" t="s" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="3">
+        <v>79</v>
+      </c>
+      <c r="B120" t="s" s="3">
+        <v>116</v>
+      </c>
+      <c r="C120" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="D120" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E120" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F120" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G120" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H120" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I120" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J120" t="s" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="4">
+        <v>80</v>
+      </c>
+      <c r="B121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="C121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="D121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="E121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="F121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="G121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="H121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="I121" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="J121" t="s" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B122" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="C122" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="D122" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="E122" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F122" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G122" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H122" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I122" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J122" t="s" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="B123" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="C123" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="D123" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="E123" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F123" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G123" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H123" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I123" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J123" t="s" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="B124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="C124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="D124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="E124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="F124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="G124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="H124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="I124" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="J124" t="s" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="B125" t="s" s="3">
+        <v>117</v>
+      </c>
+      <c r="C125" t="s" s="3">
+        <v>136</v>
+      </c>
+      <c r="D125" t="s" s="3">
+        <v>150</v>
+      </c>
+      <c r="E125" t="s" s="3">
+        <v>159</v>
+      </c>
+      <c r="F125" t="s" s="3">
+        <v>168</v>
+      </c>
+      <c r="G125" t="s" s="3">
+        <v>176</v>
+      </c>
+      <c r="H125" t="s" s="3">
+        <v>183</v>
+      </c>
+      <c r="I125" t="s" s="3">
+        <v>192</v>
+      </c>
+      <c r="J125" t="s" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="B126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="C126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="D126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="E126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="F126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="G126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="H126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="I126" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="J126" t="s" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="B127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="C127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="D127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="E127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="F127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="G127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="H127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="I127" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="J127" t="s" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="B128" t="s" s="3">
+        <v>118</v>
+      </c>
+      <c r="C128" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="D128" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="E128" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F128" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G128" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H128" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I128" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J128" t="s" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="3">
+        <v>85</v>
+      </c>
+      <c r="B129" t="s" s="3">
+        <v>119</v>
+      </c>
+      <c r="C129" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="D129" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="E129" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="F129" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G129" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="H129" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="I129" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J129" t="s" s="3">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4440,6 +4915,10 @@
     <mergeCell ref="A109:J109"/>
     <mergeCell ref="A112:J112"/>
     <mergeCell ref="A115:J115"/>
+    <mergeCell ref="A118:J118"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="A124:J124"/>
+    <mergeCell ref="A127:J127"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>